<commit_message>
Update rounding in age sampling
</commit_message>
<xml_diff>
--- a/data/vic_reference.xlsx
+++ b/data/vic_reference.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F1A306-53A0-4686-A446-C1984AF3B156}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0779042-DDFA-4907-8912-FFBB7706CC6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3810" yWindow="7665" windowWidth="28890" windowHeight="13335" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10470" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Sheet 0" sheetId="1" r:id="rId1"/>
@@ -1048,15 +1048,15 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16:B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>132</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>16</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>17</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>18</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>19</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>21</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>22</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>23</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>25</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>26</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>27</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>28</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>29</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>30</v>
       </c>
@@ -1232,1111 +1232,1111 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>31</v>
       </c>
       <c r="B17" s="12">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="C17" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>32</v>
       </c>
       <c r="B18" s="12">
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="C18" s="12">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>33</v>
       </c>
       <c r="B19" s="12">
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="C19" s="12">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="12">
-        <v>427</v>
+      <c r="B20" s="2">
+        <v>51644</v>
       </c>
       <c r="C20" s="12">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="12">
-        <v>1023</v>
+      <c r="B21" s="2">
+        <v>57082</v>
       </c>
       <c r="C21" s="12">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="12">
-        <v>1822</v>
+      <c r="B22" s="2">
+        <v>60109</v>
       </c>
       <c r="C22" s="12">
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="12">
-        <v>2859</v>
+      <c r="B23" s="2">
+        <v>62268</v>
       </c>
       <c r="C23" s="12">
         <v>128</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="12">
-        <v>3869</v>
+      <c r="B24" s="2">
+        <v>62977</v>
       </c>
       <c r="C24" s="12">
         <v>194</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="12">
-        <v>5376</v>
+      <c r="B25" s="2">
+        <v>65017</v>
       </c>
       <c r="C25" s="12">
         <v>215</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="12">
-        <v>6944</v>
+      <c r="B26" s="2">
+        <v>65748</v>
       </c>
       <c r="C26" s="12">
         <v>270</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="12">
-        <v>9489</v>
+      <c r="B27" s="2">
+        <v>67616</v>
       </c>
       <c r="C27" s="12">
         <v>320</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="12">
-        <v>11827</v>
+      <c r="B28" s="2">
+        <v>69524</v>
       </c>
       <c r="C28" s="12">
         <v>331</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="12">
-        <v>14231</v>
+      <c r="B29" s="2">
+        <v>68853</v>
       </c>
       <c r="C29" s="12">
         <v>359</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="12">
-        <v>16492</v>
+      <c r="B30" s="2">
+        <v>70349</v>
       </c>
       <c r="C30" s="12">
         <v>413</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B31" s="12">
-        <v>18451</v>
+      <c r="B31" s="2">
+        <v>69066</v>
       </c>
       <c r="C31" s="12">
         <v>403</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="12">
-        <v>20547</v>
+      <c r="B32" s="2">
+        <v>70911</v>
       </c>
       <c r="C32" s="12">
         <v>464</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B33" s="12">
-        <v>22401</v>
+      <c r="B33" s="2">
+        <v>70593</v>
       </c>
       <c r="C33" s="12">
         <v>446</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B34" s="12">
-        <v>23512</v>
+      <c r="B34" s="2">
+        <v>70290</v>
       </c>
       <c r="C34" s="12">
         <v>451</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="12">
-        <v>24904</v>
+      <c r="B35" s="2">
+        <v>70329</v>
       </c>
       <c r="C35" s="12">
         <v>492</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="12">
-        <v>24875</v>
+      <c r="B36" s="2">
+        <v>68168</v>
       </c>
       <c r="C36" s="12">
         <v>449</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B37" s="12">
-        <v>25373</v>
+      <c r="B37" s="2">
+        <v>66195</v>
       </c>
       <c r="C37" s="12">
         <v>472</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B38" s="12">
-        <v>24674</v>
+      <c r="B38" s="2">
+        <v>63651</v>
       </c>
       <c r="C38" s="12">
         <v>469</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B39" s="12">
-        <v>24265</v>
+      <c r="B39" s="2">
+        <v>61078</v>
       </c>
       <c r="C39" s="12">
         <v>482</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B40" s="12">
-        <v>23911</v>
+      <c r="B40" s="2">
+        <v>58825</v>
       </c>
       <c r="C40" s="12">
         <v>444</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B41" s="12">
-        <v>23769</v>
+      <c r="B41" s="2">
+        <v>57758</v>
       </c>
       <c r="C41" s="12">
         <v>445</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B42" s="12">
-        <v>23963</v>
+      <c r="B42" s="2">
+        <v>57888</v>
       </c>
       <c r="C42" s="12">
         <v>465</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B43" s="12">
-        <v>24296</v>
+      <c r="B43" s="2">
+        <v>57474</v>
       </c>
       <c r="C43" s="12">
         <v>495</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B44" s="12">
-        <v>24946</v>
+      <c r="B44" s="2">
+        <v>58945</v>
       </c>
       <c r="C44" s="12">
         <v>506</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B45" s="12">
-        <v>25075</v>
+      <c r="B45" s="2">
+        <v>58764</v>
       </c>
       <c r="C45" s="12">
         <v>506</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="B46" s="12">
-        <v>26130</v>
+      <c r="B46" s="2">
+        <v>60562</v>
       </c>
       <c r="C46" s="12">
         <v>556</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B47" s="12">
-        <v>26852</v>
+      <c r="B47" s="2">
+        <v>62188</v>
       </c>
       <c r="C47" s="12">
         <v>561</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="B48" s="12">
-        <v>25398</v>
+      <c r="B48" s="2">
+        <v>58516</v>
       </c>
       <c r="C48" s="12">
         <v>508</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="B49" s="12">
-        <v>24983</v>
+      <c r="B49" s="2">
+        <v>57151</v>
       </c>
       <c r="C49" s="12">
         <v>535</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B50" s="12">
-        <v>24422</v>
+      <c r="B50" s="2">
+        <v>55721</v>
       </c>
       <c r="C50" s="12">
         <v>470</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="B51" s="12">
-        <v>23133</v>
+      <c r="B51" s="2">
+        <v>52759</v>
       </c>
       <c r="C51" s="12">
         <v>444</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="B52" s="12">
-        <v>23043</v>
+      <c r="B52" s="2">
+        <v>52699</v>
       </c>
       <c r="C52" s="12">
         <v>463</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="B53" s="12">
-        <v>22281</v>
+      <c r="B53" s="2">
+        <v>51203</v>
       </c>
       <c r="C53" s="12">
         <v>458</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="B54" s="12">
-        <v>22656</v>
+      <c r="B54" s="2">
+        <v>52390</v>
       </c>
       <c r="C54" s="12">
         <v>450</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="B55" s="12">
-        <v>22376</v>
+      <c r="B55" s="2">
+        <v>52233</v>
       </c>
       <c r="C55" s="12">
         <v>481</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B56" s="12">
-        <v>21480</v>
+      <c r="B56" s="2">
+        <v>50728</v>
       </c>
       <c r="C56" s="12">
         <v>479</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="B57" s="12">
-        <v>21075</v>
+      <c r="B57" s="2">
+        <v>50400</v>
       </c>
       <c r="C57" s="12">
         <v>435</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="B58" s="12">
-        <v>19958</v>
+      <c r="B58" s="2">
+        <v>48635</v>
       </c>
       <c r="C58" s="12">
         <v>392</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="B59" s="12">
-        <v>19070</v>
+      <c r="B59" s="2">
+        <v>46799</v>
       </c>
       <c r="C59" s="12">
         <v>418</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="B60" s="12">
-        <v>18236</v>
+      <c r="B60" s="2">
+        <v>46043</v>
       </c>
       <c r="C60" s="12">
         <v>409</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="B61" s="12">
-        <v>17313</v>
+      <c r="B61" s="2">
+        <v>44144</v>
       </c>
       <c r="C61" s="12">
         <v>379</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B62" s="12">
-        <v>16983</v>
+      <c r="B62" s="2">
+        <v>44053</v>
       </c>
       <c r="C62" s="12">
         <v>334</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="B63" s="12">
-        <v>15619</v>
+      <c r="B63" s="2">
+        <v>41591</v>
       </c>
       <c r="C63" s="12">
         <v>364</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="B64" s="12">
-        <v>14989</v>
+      <c r="B64" s="2">
+        <v>40048</v>
       </c>
       <c r="C64" s="12">
         <v>350</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="B65" s="12">
-        <v>14256</v>
+      <c r="B65" s="2">
+        <v>39347</v>
       </c>
       <c r="C65" s="12">
         <v>332</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B66" s="12">
-        <v>13650</v>
+      <c r="B66" s="2">
+        <v>38105</v>
       </c>
       <c r="C66" s="12">
         <v>327</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="B67" s="12">
-        <v>13417</v>
+      <c r="B67" s="2">
+        <v>37557</v>
       </c>
       <c r="C67" s="12">
         <v>331</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="B68" s="12">
-        <v>12779</v>
+      <c r="B68" s="2">
+        <v>36069</v>
       </c>
       <c r="C68" s="12">
         <v>326</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="B69" s="12">
-        <v>12432</v>
+      <c r="B69" s="2">
+        <v>35044</v>
       </c>
       <c r="C69" s="12">
         <v>309</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="B70" s="12">
-        <v>12232</v>
+      <c r="B70" s="2">
+        <v>35468</v>
       </c>
       <c r="C70" s="12">
         <v>268</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="B71" s="12">
-        <v>13009</v>
+      <c r="B71" s="2">
+        <v>36916</v>
       </c>
       <c r="C71" s="12">
         <v>339</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="B72" s="12">
-        <v>10839</v>
+      <c r="B72" s="2">
+        <v>30984</v>
       </c>
       <c r="C72" s="12">
         <v>283</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="B73" s="12">
-        <v>9917</v>
+      <c r="B73" s="2">
+        <v>28539</v>
       </c>
       <c r="C73" s="12">
         <v>241</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="B74" s="12">
-        <v>9586</v>
+      <c r="B74" s="2">
+        <v>27857</v>
       </c>
       <c r="C74" s="12">
         <v>192</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="B75" s="12">
-        <v>8559</v>
+      <c r="B75" s="2">
+        <v>24576</v>
       </c>
       <c r="C75" s="12">
         <v>199</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="B76" s="12">
-        <v>8501</v>
+      <c r="B76" s="2">
+        <v>24515</v>
       </c>
       <c r="C76" s="12">
         <v>220</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B77" s="12">
-        <v>7820</v>
+      <c r="B77" s="2">
+        <v>22998</v>
       </c>
       <c r="C77" s="12">
         <v>190</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="B78" s="12">
-        <v>7680</v>
+      <c r="B78" s="2">
+        <v>22513</v>
       </c>
       <c r="C78" s="12">
         <v>180</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="B79" s="12">
-        <v>7075</v>
+      <c r="B79" s="2">
+        <v>21180</v>
       </c>
       <c r="C79" s="12">
         <v>190</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="B80" s="12">
-        <v>6783</v>
+      <c r="B80" s="2">
+        <v>20299</v>
       </c>
       <c r="C80" s="12">
         <v>161</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="B81" s="12">
-        <v>6249</v>
+      <c r="B81" s="2">
+        <v>19183</v>
       </c>
       <c r="C81" s="12">
         <v>147</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="B82" s="12">
-        <v>5889</v>
+      <c r="B82" s="2">
+        <v>18359</v>
       </c>
       <c r="C82" s="12">
         <v>148</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="B83" s="12">
-        <v>5327</v>
+      <c r="B83" s="2">
+        <v>16639</v>
       </c>
       <c r="C83" s="12">
         <v>107</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="B84" s="12">
-        <v>5044</v>
+      <c r="B84" s="2">
+        <v>15860</v>
       </c>
       <c r="C84" s="12">
         <v>137</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="B85" s="12">
-        <v>4484</v>
+      <c r="B85" s="2">
+        <v>14577</v>
       </c>
       <c r="C85" s="12">
         <v>120</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="B86" s="12">
-        <v>3910</v>
+      <c r="B86" s="2">
+        <v>13563</v>
       </c>
       <c r="C86" s="12">
         <v>92</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="B87" s="12">
-        <v>3712</v>
+      <c r="B87" s="2">
+        <v>13090</v>
       </c>
       <c r="C87" s="12">
         <v>78</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="B88" s="12">
-        <v>3272</v>
+      <c r="B88" s="2">
+        <v>12411</v>
       </c>
       <c r="C88" s="12">
         <v>92</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="B89" s="12">
-        <v>2677</v>
+      <c r="B89" s="2">
+        <v>10625</v>
       </c>
       <c r="C89" s="12">
         <v>63</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="B90" s="12">
-        <v>2231</v>
+      <c r="B90" s="2">
+        <v>9448</v>
       </c>
       <c r="C90" s="12">
         <v>42</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="B91" s="12">
-        <v>1889</v>
+      <c r="B91" s="2">
+        <v>8392</v>
       </c>
       <c r="C91" s="12">
         <v>37</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="B92" s="12">
-        <v>1481</v>
+      <c r="B92" s="2">
+        <v>7237</v>
       </c>
       <c r="C92" s="12">
         <v>42</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="B93" s="12">
-        <v>1062</v>
+      <c r="B93" s="2">
+        <v>5790</v>
       </c>
       <c r="C93" s="12">
         <v>39</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="B94" s="12">
-        <v>849</v>
+      <c r="B94" s="2">
+        <v>4815</v>
       </c>
       <c r="C94" s="12">
         <v>17</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="B95" s="12">
-        <v>593</v>
+      <c r="B95" s="2">
+        <v>3856</v>
       </c>
       <c r="C95" s="12">
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="B96" s="12">
-        <v>419</v>
+      <c r="B96" s="2">
+        <v>2895</v>
       </c>
       <c r="C96" s="12">
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="B97" s="12">
-        <v>319</v>
+      <c r="B97" s="2">
+        <v>2330</v>
       </c>
       <c r="C97" s="12">
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="B98" s="12">
-        <v>215</v>
+      <c r="B98" s="2">
+        <v>1584</v>
       </c>
       <c r="C98" s="12">
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="B99" s="12">
-        <v>105</v>
+      <c r="B99" s="2">
+        <v>903</v>
       </c>
       <c r="C99" s="12">
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="B100" s="12">
-        <v>92</v>
+      <c r="B100" s="2">
+        <v>684</v>
       </c>
       <c r="C100" s="12">
         <v>6</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="B101" s="12">
-        <v>51</v>
+      <c r="B101" s="2">
+        <v>480</v>
       </c>
       <c r="C101" s="12">
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="B102" s="12">
-        <v>24</v>
+      <c r="B102" s="2">
+        <v>260</v>
       </c>
       <c r="C102" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="B103" s="12">
-        <v>8</v>
+      <c r="B103" s="2">
+        <v>184</v>
       </c>
       <c r="C103" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="B104" s="12">
-        <v>3</v>
+      <c r="B104" s="2">
+        <v>107</v>
       </c>
       <c r="C104" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="B105" s="12">
-        <v>3</v>
+      <c r="B105" s="2">
+        <v>62</v>
       </c>
       <c r="C105" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="B106" s="12">
-        <v>0</v>
+      <c r="B106" s="2">
+        <v>40</v>
       </c>
       <c r="C106" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="B107" s="12">
-        <v>0</v>
+      <c r="B107" s="2">
+        <v>29</v>
       </c>
       <c r="C107" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="B108" s="12">
-        <v>0</v>
+      <c r="B108" s="2">
+        <v>9</v>
       </c>
       <c r="C108" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="B109" s="12">
-        <v>0</v>
+      <c r="B109" s="2">
+        <v>5</v>
       </c>
       <c r="C109" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="B110" s="12">
-        <v>0</v>
+      <c r="B110" s="2">
+        <v>6</v>
       </c>
       <c r="C110" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="B111" s="12">
+      <c r="B111" s="2">
         <v>0</v>
       </c>
       <c r="C111" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="B112" s="12">
-        <v>0</v>
+      <c r="B112" s="2">
+        <v>3</v>
       </c>
       <c r="C112" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="B113" s="12">
+      <c r="B113" s="2">
         <v>0</v>
       </c>
       <c r="C113" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="B114" s="12">
+      <c r="B114" s="2">
         <v>0</v>
       </c>
       <c r="C114" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="B115" s="12">
-        <v>0</v>
+      <c r="B115" s="2">
+        <v>4</v>
       </c>
       <c r="C115" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="B116" s="12">
-        <v>0</v>
+      <c r="B116" s="2">
+        <v>3</v>
       </c>
       <c r="C116" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="B117" s="12">
+      <c r="B117" s="2">
         <v>0</v>
       </c>
       <c r="C117" s="12">
@@ -2345,113 +2345,6 @@
     </row>
   </sheetData>
   <mergeCells count="118">
-    <mergeCell ref="A2"/>
-    <mergeCell ref="A3"/>
-    <mergeCell ref="A4"/>
-    <mergeCell ref="A5"/>
-    <mergeCell ref="A6"/>
-    <mergeCell ref="B1"/>
-    <mergeCell ref="C1"/>
-    <mergeCell ref="A12"/>
-    <mergeCell ref="A13"/>
-    <mergeCell ref="A14"/>
-    <mergeCell ref="A15"/>
-    <mergeCell ref="A16"/>
-    <mergeCell ref="A7"/>
-    <mergeCell ref="A8"/>
-    <mergeCell ref="A9"/>
-    <mergeCell ref="A10"/>
-    <mergeCell ref="A11"/>
-    <mergeCell ref="A22"/>
-    <mergeCell ref="A23"/>
-    <mergeCell ref="A24"/>
-    <mergeCell ref="A25"/>
-    <mergeCell ref="A26"/>
-    <mergeCell ref="A17"/>
-    <mergeCell ref="A18"/>
-    <mergeCell ref="A19"/>
-    <mergeCell ref="A20"/>
-    <mergeCell ref="A21"/>
-    <mergeCell ref="A32"/>
-    <mergeCell ref="A33"/>
-    <mergeCell ref="A34"/>
-    <mergeCell ref="A35"/>
-    <mergeCell ref="A36"/>
-    <mergeCell ref="A27"/>
-    <mergeCell ref="A28"/>
-    <mergeCell ref="A29"/>
-    <mergeCell ref="A30"/>
-    <mergeCell ref="A31"/>
-    <mergeCell ref="A42"/>
-    <mergeCell ref="A43"/>
-    <mergeCell ref="A44"/>
-    <mergeCell ref="A45"/>
-    <mergeCell ref="A46"/>
-    <mergeCell ref="A37"/>
-    <mergeCell ref="A38"/>
-    <mergeCell ref="A39"/>
-    <mergeCell ref="A40"/>
-    <mergeCell ref="A41"/>
-    <mergeCell ref="A52"/>
-    <mergeCell ref="A53"/>
-    <mergeCell ref="A54"/>
-    <mergeCell ref="A55"/>
-    <mergeCell ref="A56"/>
-    <mergeCell ref="A47"/>
-    <mergeCell ref="A48"/>
-    <mergeCell ref="A49"/>
-    <mergeCell ref="A50"/>
-    <mergeCell ref="A51"/>
-    <mergeCell ref="A62"/>
-    <mergeCell ref="A63"/>
-    <mergeCell ref="A64"/>
-    <mergeCell ref="A65"/>
-    <mergeCell ref="A66"/>
-    <mergeCell ref="A57"/>
-    <mergeCell ref="A58"/>
-    <mergeCell ref="A59"/>
-    <mergeCell ref="A60"/>
-    <mergeCell ref="A61"/>
-    <mergeCell ref="A72"/>
-    <mergeCell ref="A73"/>
-    <mergeCell ref="A74"/>
-    <mergeCell ref="A75"/>
-    <mergeCell ref="A76"/>
-    <mergeCell ref="A67"/>
-    <mergeCell ref="A68"/>
-    <mergeCell ref="A69"/>
-    <mergeCell ref="A70"/>
-    <mergeCell ref="A71"/>
-    <mergeCell ref="A82"/>
-    <mergeCell ref="A83"/>
-    <mergeCell ref="A84"/>
-    <mergeCell ref="A85"/>
-    <mergeCell ref="A86"/>
-    <mergeCell ref="A77"/>
-    <mergeCell ref="A78"/>
-    <mergeCell ref="A79"/>
-    <mergeCell ref="A80"/>
-    <mergeCell ref="A81"/>
-    <mergeCell ref="A92"/>
-    <mergeCell ref="A93"/>
-    <mergeCell ref="A94"/>
-    <mergeCell ref="A95"/>
-    <mergeCell ref="A96"/>
-    <mergeCell ref="A87"/>
-    <mergeCell ref="A88"/>
-    <mergeCell ref="A89"/>
-    <mergeCell ref="A90"/>
-    <mergeCell ref="A91"/>
-    <mergeCell ref="A102"/>
-    <mergeCell ref="A103"/>
-    <mergeCell ref="A104"/>
-    <mergeCell ref="A105"/>
-    <mergeCell ref="A106"/>
-    <mergeCell ref="A97"/>
-    <mergeCell ref="A98"/>
-    <mergeCell ref="A99"/>
-    <mergeCell ref="A100"/>
-    <mergeCell ref="A101"/>
     <mergeCell ref="A117"/>
     <mergeCell ref="A112"/>
     <mergeCell ref="A113"/>
@@ -2463,6 +2356,113 @@
     <mergeCell ref="A109"/>
     <mergeCell ref="A110"/>
     <mergeCell ref="A111"/>
+    <mergeCell ref="A102"/>
+    <mergeCell ref="A103"/>
+    <mergeCell ref="A104"/>
+    <mergeCell ref="A105"/>
+    <mergeCell ref="A106"/>
+    <mergeCell ref="A97"/>
+    <mergeCell ref="A98"/>
+    <mergeCell ref="A99"/>
+    <mergeCell ref="A100"/>
+    <mergeCell ref="A101"/>
+    <mergeCell ref="A92"/>
+    <mergeCell ref="A93"/>
+    <mergeCell ref="A94"/>
+    <mergeCell ref="A95"/>
+    <mergeCell ref="A96"/>
+    <mergeCell ref="A87"/>
+    <mergeCell ref="A88"/>
+    <mergeCell ref="A89"/>
+    <mergeCell ref="A90"/>
+    <mergeCell ref="A91"/>
+    <mergeCell ref="A82"/>
+    <mergeCell ref="A83"/>
+    <mergeCell ref="A84"/>
+    <mergeCell ref="A85"/>
+    <mergeCell ref="A86"/>
+    <mergeCell ref="A77"/>
+    <mergeCell ref="A78"/>
+    <mergeCell ref="A79"/>
+    <mergeCell ref="A80"/>
+    <mergeCell ref="A81"/>
+    <mergeCell ref="A72"/>
+    <mergeCell ref="A73"/>
+    <mergeCell ref="A74"/>
+    <mergeCell ref="A75"/>
+    <mergeCell ref="A76"/>
+    <mergeCell ref="A67"/>
+    <mergeCell ref="A68"/>
+    <mergeCell ref="A69"/>
+    <mergeCell ref="A70"/>
+    <mergeCell ref="A71"/>
+    <mergeCell ref="A62"/>
+    <mergeCell ref="A63"/>
+    <mergeCell ref="A64"/>
+    <mergeCell ref="A65"/>
+    <mergeCell ref="A66"/>
+    <mergeCell ref="A57"/>
+    <mergeCell ref="A58"/>
+    <mergeCell ref="A59"/>
+    <mergeCell ref="A60"/>
+    <mergeCell ref="A61"/>
+    <mergeCell ref="A52"/>
+    <mergeCell ref="A53"/>
+    <mergeCell ref="A54"/>
+    <mergeCell ref="A55"/>
+    <mergeCell ref="A56"/>
+    <mergeCell ref="A47"/>
+    <mergeCell ref="A48"/>
+    <mergeCell ref="A49"/>
+    <mergeCell ref="A50"/>
+    <mergeCell ref="A51"/>
+    <mergeCell ref="A42"/>
+    <mergeCell ref="A43"/>
+    <mergeCell ref="A44"/>
+    <mergeCell ref="A45"/>
+    <mergeCell ref="A46"/>
+    <mergeCell ref="A37"/>
+    <mergeCell ref="A38"/>
+    <mergeCell ref="A39"/>
+    <mergeCell ref="A40"/>
+    <mergeCell ref="A41"/>
+    <mergeCell ref="A32"/>
+    <mergeCell ref="A33"/>
+    <mergeCell ref="A34"/>
+    <mergeCell ref="A35"/>
+    <mergeCell ref="A36"/>
+    <mergeCell ref="A27"/>
+    <mergeCell ref="A28"/>
+    <mergeCell ref="A29"/>
+    <mergeCell ref="A30"/>
+    <mergeCell ref="A31"/>
+    <mergeCell ref="A23"/>
+    <mergeCell ref="A24"/>
+    <mergeCell ref="A25"/>
+    <mergeCell ref="A26"/>
+    <mergeCell ref="A17"/>
+    <mergeCell ref="A18"/>
+    <mergeCell ref="A19"/>
+    <mergeCell ref="A20"/>
+    <mergeCell ref="A21"/>
+    <mergeCell ref="A14"/>
+    <mergeCell ref="A15"/>
+    <mergeCell ref="A16"/>
+    <mergeCell ref="A7"/>
+    <mergeCell ref="A8"/>
+    <mergeCell ref="A9"/>
+    <mergeCell ref="A10"/>
+    <mergeCell ref="A11"/>
+    <mergeCell ref="A22"/>
+    <mergeCell ref="A2"/>
+    <mergeCell ref="A3"/>
+    <mergeCell ref="A4"/>
+    <mergeCell ref="A5"/>
+    <mergeCell ref="A6"/>
+    <mergeCell ref="B1"/>
+    <mergeCell ref="C1"/>
+    <mergeCell ref="A12"/>
+    <mergeCell ref="A13"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2480,33 +2480,33 @@
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" s="9" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" s="9" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>12</v>
       </c>
@@ -2528,42 +2528,42 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
     </row>
   </sheetData>

</xml_diff>